<commit_message>
test triangle  table complete. all test passed
</commit_message>
<xml_diff>
--- a/tests/test_plan_triangle.xlsx
+++ b/tests/test_plan_triangle.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lauri\Desktop\Intermediate Software Development0315\8. Activities\Module_02\given_files\activity_2\activity_2\tests\shape\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ralph\OneDrive - Red River College Polytech\Desktop\Intermidiate_Software_Development\Activities\Vitug_Ralph_Activity_02\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B82F31A6-8AFA-4B46-AE54-0E71FA70719A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BB12156-9629-4C26-900A-D935AB135DCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8D9DD509-55B1-455D-8036-16809AD15960}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{8D9DD509-55B1-455D-8036-16809AD15960}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -183,7 +183,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="37">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -249,6 +249,54 @@
   </si>
   <si>
     <t>calculate_perimeter</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Triangle("red",  3,  4 ,5)</t>
+  </si>
+  <si>
+    <t>Triangle("",  3,  4 ,5)</t>
+  </si>
+  <si>
+    <t>Triangle("red",  "a",  4 ,5)</t>
+  </si>
+  <si>
+    <t>Triangle("red",  3,  "b" ,5)</t>
+  </si>
+  <si>
+    <t>Triangle("red",  3,  4 ,"c")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Object created </t>
+  </si>
+  <si>
+    <t>ValueError</t>
+  </si>
+  <si>
+    <t>(3 + 4 + 5) / 2 = 6</t>
+  </si>
+  <si>
+    <t>3 + 4 + 5 = 12</t>
+  </si>
+  <si>
+    <t>12, self.triangle.calculate_perimeter()</t>
+  </si>
+  <si>
+    <t>6, self.triangle.calculate_area()</t>
+  </si>
+  <si>
+    <t>Ralph Vitug</t>
+  </si>
+  <si>
+    <t>"The shape color is red"
+"This triangle has three sides with the lengths of 3, 4 and 5 centimeters"</t>
+  </si>
+  <si>
+    <t>"The shape color is red.\n"
+            "This triangle has three sides with the lengths of "
+            "3, 4 and 5 centimeters"</t>
   </si>
 </sst>
 </file>
@@ -503,7 +551,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -552,6 +600,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1109,22 +1160,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DADEBCC4-BB44-48CD-B9AB-1E2FD3EE0EEB}">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" customWidth="1"/>
-    <col min="4" max="4" width="32.7109375" customWidth="1"/>
-    <col min="5" max="5" width="29.140625" customWidth="1"/>
-    <col min="6" max="6" width="35.42578125" customWidth="1"/>
-    <col min="7" max="7" width="26.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12.7265625" customWidth="1"/>
+    <col min="3" max="3" width="22.26953125" customWidth="1"/>
+    <col min="4" max="4" width="32.7265625" customWidth="1"/>
+    <col min="5" max="5" width="29.1796875" customWidth="1"/>
+    <col min="6" max="6" width="35.453125" customWidth="1"/>
+    <col min="7" max="7" width="26.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:7" ht="73.150000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="1.45">
+    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="1:7" ht="73.150000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="2.15">
       <c r="B2" s="2" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
@@ -1136,14 +1187,16 @@
       <c r="F2" s="14"/>
       <c r="G2" s="14"/>
     </row>
-    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="15"/>
+      <c r="C3" s="15" t="s">
+        <v>34</v>
+      </c>
       <c r="D3" s="16"/>
     </row>
-    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="6" t="s">
         <v>3</v>
       </c>
@@ -1152,10 +1205,10 @@
       </c>
       <c r="D4" s="18"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B5" s="1"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B6" s="7" t="s">
         <v>0</v>
       </c>
@@ -1175,7 +1228,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="78" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="78" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4"/>
       <c r="B7" s="11">
         <v>1</v>
@@ -1186,11 +1239,17 @@
       <c r="D7" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-    </row>
-    <row r="8" spans="1:7" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E7" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="66.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4"/>
       <c r="B8" s="12">
         <v>2</v>
@@ -1201,11 +1260,17 @@
       <c r="D8" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-    </row>
-    <row r="9" spans="1:7" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E8" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="74.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="4"/>
       <c r="B9" s="12">
         <v>3</v>
@@ -1216,11 +1281,17 @@
       <c r="D9" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-    </row>
-    <row r="10" spans="1:7" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E9" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="78.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4"/>
       <c r="B10" s="11">
         <v>4</v>
@@ -1231,11 +1302,17 @@
       <c r="D10" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-    </row>
-    <row r="11" spans="1:7" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E10" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="72" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="12">
         <v>5</v>
       </c>
@@ -1245,11 +1322,17 @@
       <c r="D11" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-    </row>
-    <row r="12" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E11" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="12">
         <v>6</v>
       </c>
@@ -1259,11 +1342,17 @@
       <c r="D12" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-    </row>
-    <row r="13" spans="1:7" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E12" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="11">
         <v>7</v>
       </c>
@@ -1273,11 +1362,17 @@
       <c r="D13" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-    </row>
-    <row r="14" spans="1:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E13" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="11">
         <v>8</v>
       </c>
@@ -1287,11 +1382,17 @@
       <c r="D14" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-    </row>
-    <row r="15" spans="1:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E14" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="F14" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="12">
         <v>9</v>
       </c>
@@ -1301,7 +1402,7 @@
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
     </row>
-    <row r="16" spans="1:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="12">
         <v>10</v>
       </c>
@@ -1311,7 +1412,7 @@
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
     </row>
-    <row r="17" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="11">
         <v>11</v>
       </c>
@@ -1321,7 +1422,7 @@
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
     </row>
-    <row r="18" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="12">
         <v>12</v>
       </c>
@@ -1331,7 +1432,7 @@
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
     </row>
-    <row r="19" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" s="12">
         <v>13</v>
       </c>
@@ -1341,7 +1442,7 @@
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
     </row>
-    <row r="20" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B20" s="11">
         <v>14</v>
       </c>
@@ -1351,7 +1452,7 @@
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
     </row>
-    <row r="21" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B21" s="11">
         <v>15</v>
       </c>
@@ -1361,7 +1462,7 @@
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
     </row>
-    <row r="22" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B22" s="12">
         <v>16</v>
       </c>
@@ -1371,7 +1472,7 @@
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
     </row>
-    <row r="23" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B23" s="12">
         <v>17</v>
       </c>
@@ -1381,7 +1482,7 @@
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
     </row>
-    <row r="24" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B24" s="11">
         <v>18</v>
       </c>
@@ -1391,7 +1492,7 @@
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B26" s="19" t="s">
         <v>6</v>
       </c>

</xml_diff>